<commit_message>
MVC with Servlets and JSP - Part 1 - Create Student Class
</commit_message>
<xml_diff>
--- a/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
+++ b/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E709C678-7845-4125-9922-82D08A3370BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86275005-EA92-48E6-9833-EAFAA2C6AB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mô hình MVC" sheetId="1" r:id="rId1"/>
     <sheet name="Servlets and JSP Simple" sheetId="2" r:id="rId2"/>
+    <sheet name="Sơ đồ" sheetId="3" r:id="rId3"/>
+    <sheet name="Create Student Class" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Add JSTL support to servletdemo project</t>
   </si>
@@ -44,6 +46,18 @@
   </si>
   <si>
     <t>http://localhost:8080/servletdemo/MvcDemoServlet</t>
+  </si>
+  <si>
+    <t>Create mvctwo package</t>
+  </si>
+  <si>
+    <t>Create Student Class</t>
+  </si>
+  <si>
+    <t>Create Constructor</t>
+  </si>
+  <si>
+    <t>Generate Getters and Setters</t>
   </si>
 </sst>
 </file>
@@ -544,6 +558,544 @@
         <a:xfrm>
           <a:off x="609600" y="40576500"/>
           <a:ext cx="4885714" cy="1704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>160457</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>75643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3106B16-4BCA-458B-8728-BB72C859F582}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="11742857" cy="4457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46781</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E98C614F-A16E-47E6-9802-F86153A25126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="6752381" cy="5019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>599467</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE20E944-4B70-4C11-AF27-9C20DD78CF0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="4866667" cy="4076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9143</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>28143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60F2F602-82D0-476B-8940-60A128378160}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9906000"/>
+          <a:ext cx="3057143" cy="3457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>389562</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>8905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31443CD3-A80A-4A3A-AD5E-C548AAA5B98A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="13716000"/>
+          <a:ext cx="7704762" cy="4961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>151771</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>104024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{781E70B1-E453-4748-AB00-BA33A9B59729}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="18859500"/>
+          <a:ext cx="5028571" cy="6009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>237333</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>190048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB9708B7-72E4-44F1-9DAD-B85AA370D24E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="25146000"/>
+          <a:ext cx="6333333" cy="3619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>55848</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>170929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACDD708-7890-44B5-9A0B-E552255DABFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="29337000"/>
+          <a:ext cx="10419048" cy="4171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>513752</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>113500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6FF9EB4-5EDA-4970-96D4-2C9B1BDB5831}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="33718500"/>
+          <a:ext cx="4780952" cy="6400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>608228</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>66048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3486517C-0157-4160-A793-E4699FA4C386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="40576500"/>
+          <a:ext cx="10971428" cy="5019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>570895</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>84905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A1E05E1-E9AB-4B8A-9F52-C98E573F727A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="45720000"/>
+          <a:ext cx="4838095" cy="6561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>199009</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>56405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81E1859-A420-40C5-8488-083D178BD3D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52578000"/>
+          <a:ext cx="8123809" cy="5961905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -835,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2DBBAD-0387-4A1A-982F-E27CF7EC679F}">
   <dimension ref="A2:B213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="O214" sqref="O214"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="N131" sqref="N131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,4 +1427,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E0C26-FAC7-4394-B3E6-2866D1844922}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A563C8-6AD7-4C1A-8016-279DC78294A8}">
+  <dimension ref="A2:A213"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MVC with Servlets and JSP - Part 2 - Create StudentDataUtil(Model)
</commit_message>
<xml_diff>
--- a/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
+++ b/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86275005-EA92-48E6-9833-EAFAA2C6AB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4C518-7AA5-490F-9260-9AF70D4A4E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mô hình MVC" sheetId="1" r:id="rId1"/>
     <sheet name="Servlets and JSP Simple" sheetId="2" r:id="rId2"/>
     <sheet name="Sơ đồ" sheetId="3" r:id="rId3"/>
     <sheet name="Create Student Class" sheetId="4" r:id="rId4"/>
+    <sheet name="Create StudentDataUtil(Model)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Add JSTL support to servletdemo project</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>Generate Getters and Setters</t>
+  </si>
+  <si>
+    <t>Create StudentDataUtil</t>
   </si>
 </sst>
 </file>
@@ -1096,6 +1100,143 @@
         <a:xfrm>
           <a:off x="609600" y="52578000"/>
           <a:ext cx="8123809" cy="5961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>122895</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>151762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF7CBE46-8C35-49D4-A300-A29BECC78750}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="7438095" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>161295</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>123071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BC2BBB-D272-41FC-8720-D21810FE8F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="5038095" cy="6028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>408533</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>142357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450C42B1-9CE3-41AF-B34C-A1E564A71B69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="12001500"/>
+          <a:ext cx="8333333" cy="4142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1448,7 +1589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A563C8-6AD7-4C1A-8016-279DC78294A8}">
   <dimension ref="A2:A213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+    <sheetView topLeftCell="A298" workbookViewId="0">
       <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
@@ -1478,4 +1619,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC4AB73-B2BC-45A9-8094-C02C57C1DA39}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MVC with Servlets and JSP - Part 3 - Create MVC Servlet(Controller)
</commit_message>
<xml_diff>
--- a/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
+++ b/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4C518-7AA5-490F-9260-9AF70D4A4E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43041300-4F7C-4CEA-927E-A8F798A87662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mô hình MVC" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sơ đồ" sheetId="3" r:id="rId3"/>
     <sheet name="Create Student Class" sheetId="4" r:id="rId4"/>
     <sheet name="Create StudentDataUtil(Model)" sheetId="5" r:id="rId5"/>
+    <sheet name="Create MVC Servlet(Controller)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Add JSTL support to servletdemo project</t>
   </si>
@@ -62,6 +63,9 @@
   </si>
   <si>
     <t>Create StudentDataUtil</t>
+  </si>
+  <si>
+    <t>Create MvcDemoServletTwo(Controller)</t>
   </si>
 </sst>
 </file>
@@ -1237,6 +1241,143 @@
         <a:xfrm>
           <a:off x="609600" y="12001500"/>
           <a:ext cx="8333333" cy="4142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>265752</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>151762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20494574-0FD7-4BE9-9593-C00B4072606A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="7580952" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9972A46C-84AE-411A-A3B7-E745BE0F65D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5715000"/>
+          <a:ext cx="4876190" cy="3609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8076</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>37357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{533F9E68-281E-4644-BA79-52ECDD1AAB54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9525000"/>
+          <a:ext cx="11590476" cy="5942857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1574,7 +1715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E0C26-FAC7-4394-B3E6-2866D1844922}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC4AB73-B2BC-45A9-8094-C02C57C1DA39}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
@@ -1640,4 +1781,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED552179-9AFC-498B-A038-961D70A9852A}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MVC with Servlets and JSP - Part 4 - Create JSP View with HTML Tables
</commit_message>
<xml_diff>
--- a/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
+++ b/me_docs/9.Build-an-MVC-App-with-Servlets-and-JSP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43041300-4F7C-4CEA-927E-A8F798A87662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E10999E-E124-4D15-8BCF-EFD3F72B377F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mô hình MVC" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Create Student Class" sheetId="4" r:id="rId4"/>
     <sheet name="Create StudentDataUtil(Model)" sheetId="5" r:id="rId5"/>
     <sheet name="Create MVC Servlet(Controller)" sheetId="6" r:id="rId6"/>
+    <sheet name="Create JSP View" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Add JSTL support to servletdemo project</t>
   </si>
@@ -66,6 +67,18 @@
   </si>
   <si>
     <t>Create MvcDemoServletTwo(Controller)</t>
+  </si>
+  <si>
+    <t>create view_students_two.jsp</t>
+  </si>
+  <si>
+    <t>Run Server</t>
+  </si>
+  <si>
+    <t>Create index.html</t>
+  </si>
+  <si>
+    <t>Run Server again</t>
   </si>
 </sst>
 </file>
@@ -1378,6 +1391,495 @@
         <a:xfrm>
           <a:off x="609600" y="9525000"/>
           <a:ext cx="11590476" cy="5942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>37181</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>18429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D99EB28-D499-41F1-9399-881A07ADD0B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="7352381" cy="4971429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3563E4A-671D-47A0-87D4-98711ED3A360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="4857143" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>303848</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>56476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1CACC89-B2FD-4056-9135-AECC5CA9F092}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11430000"/>
+          <a:ext cx="7619048" cy="5390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>446857</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>170809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F1718CD-17B9-4D61-995A-4FE918EBDBF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17335500"/>
+          <a:ext cx="6542857" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>37786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FC6233B-6C79-4D30-A6F4-50F57C564B87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="22669500"/>
+          <a:ext cx="4885714" cy="2514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>8686</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>180333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F79FFF19-E23D-42B6-816B-C1694C15862C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="25527000"/>
+          <a:ext cx="6714286" cy="5133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>170738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7204EDE4-AC14-4847-962A-4D5CC6EBC523}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="30861000"/>
+          <a:ext cx="4876190" cy="5695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>513448</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>104095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C9FD88-E1EA-4751-997E-C8B626CF2A44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="36766500"/>
+          <a:ext cx="7219048" cy="5438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>446857</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>170809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B29AF6-581A-4FE9-9AEB-A0E60BD90700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="42672000"/>
+          <a:ext cx="6542857" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285257</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>85524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AE128D-6073-44A6-8502-7D50B4F0FE2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="48006000"/>
+          <a:ext cx="3942857" cy="1609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>133024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B184F702-8E23-4863-AD06-788795648849}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="49911000"/>
+          <a:ext cx="4895238" cy="2609524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1787,7 +2289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED552179-9AFC-498B-A038-961D70A9852A}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -1802,4 +2304,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6003EA6-DD51-4359-9187-2EAD89F2EDB5}">
+  <dimension ref="A2:A224"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>